<commit_message>
Adjustment of energy sources for Danish units
</commit_message>
<xml_diff>
--- a/input/input_plant-list_DK.xlsx
+++ b/input/input_plant-list_DK.xlsx
@@ -148,9 +148,6 @@
     <t>45V0000000000172</t>
   </si>
   <si>
-    <t>UNKNOWN</t>
-  </si>
-  <si>
     <t>Biomass and biogas</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>Zone: West (DK1)</t>
+  </si>
+  <si>
+    <t>Other or unspecified energy sources</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,61 +625,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -687,16 +687,16 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="1">
         <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M2">
         <v>2009</v>
@@ -722,16 +722,16 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="1">
         <v>265</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M3">
         <v>1989</v>
@@ -757,16 +757,16 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" s="1">
         <v>140</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M4">
         <v>1961</v>
@@ -792,16 +792,16 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="1">
         <v>665</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M5">
         <v>1981</v>
@@ -827,16 +827,16 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G6" s="1">
         <v>265</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M6">
         <v>1990</v>
@@ -862,16 +862,16 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" s="1">
         <v>545</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M7">
         <v>2002</v>
@@ -897,19 +897,19 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" s="1">
         <v>665</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M8">
         <v>1979</v>
@@ -935,16 +935,16 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" s="1">
         <v>400</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M9">
         <v>1992</v>
@@ -970,19 +970,19 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" s="1">
         <v>410</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M10">
         <v>1991</v>
@@ -1008,16 +1008,16 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" s="1">
         <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M11">
         <v>2009</v>
@@ -1043,16 +1043,16 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" s="1">
         <v>75</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M12">
         <v>1985</v>
@@ -1075,16 +1075,16 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G13" s="1">
         <v>25</v>
       </c>
       <c r="H13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M13">
         <v>2004</v>
@@ -1107,16 +1107,16 @@
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" s="1">
         <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M14">
         <v>1954</v>
@@ -1139,16 +1139,16 @@
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" s="1">
         <v>90</v>
       </c>
       <c r="H15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M15">
         <v>1982</v>
@@ -1171,16 +1171,16 @@
         <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G16" s="1">
         <v>260</v>
       </c>
       <c r="H16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M16">
         <v>1974</v>
@@ -1206,16 +1206,16 @@
         <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="1">
         <v>260</v>
       </c>
       <c r="H17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M17">
         <v>1976</v>
@@ -1241,16 +1241,16 @@
         <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="1">
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M18">
         <v>1974</v>
@@ -1276,16 +1276,16 @@
         <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G19" s="1">
         <v>125</v>
       </c>
       <c r="H19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M19">
         <v>1973</v>
@@ -1311,16 +1311,16 @@
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G20" s="1">
         <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="J20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M20">
         <v>1975</v>
@@ -1343,19 +1343,19 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G21" s="1">
         <v>25</v>
       </c>
       <c r="H21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M21">
         <v>1976</v>
@@ -1381,19 +1381,19 @@
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G22" s="1">
         <v>220</v>
       </c>
       <c r="H22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M22">
         <v>1977</v>
@@ -1419,19 +1419,19 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G23" s="1">
         <v>410</v>
       </c>
       <c r="H23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M23">
         <v>1998</v>
@@ -1457,16 +1457,16 @@
         <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G24" s="1">
         <v>90</v>
       </c>
       <c r="H24" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="J24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M24">
         <v>2014</v>
@@ -1489,16 +1489,16 @@
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G25" s="1">
         <v>430</v>
       </c>
       <c r="H25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M25">
         <v>1997</v>
@@ -1524,16 +1524,16 @@
         <v>31</v>
       </c>
       <c r="F26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G26" s="1">
         <v>265</v>
       </c>
       <c r="H26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M26">
         <v>1970</v>
@@ -1559,19 +1559,19 @@
         <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G27" s="1">
         <v>380</v>
       </c>
       <c r="H27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M27">
         <v>1984</v>
@@ -1597,19 +1597,19 @@
         <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G28" s="1">
         <v>380</v>
       </c>
       <c r="H28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M28">
         <v>1985</v>
@@ -1635,19 +1635,19 @@
         <v>6</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G29" s="1">
         <v>15</v>
       </c>
       <c r="H29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M29">
         <v>1986</v>
@@ -1673,16 +1673,16 @@
         <v>29</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G30" s="1">
         <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M30">
         <v>1953</v>
@@ -1705,16 +1705,16 @@
         <v>30</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G31" s="1">
         <v>60</v>
       </c>
       <c r="H31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M31">
         <v>1995</v>

</xml_diff>